<commit_message>
Added test case data
</commit_message>
<xml_diff>
--- a/testData/SurveyMultiGood.xlsx
+++ b/testData/SurveyMultiGood.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="A2:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>